<commit_message>
8th - Tickets index page implements jq-datatables
Allows selection by dropdown list, limits tickets displayed by role
</commit_message>
<xml_diff>
--- a/BugTracker-classes.xlsx
+++ b/BugTracker-classes.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22290" windowHeight="7710"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="22290" windowHeight="7710"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Classes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
   <si>
     <t>Ticket</t>
   </si>
@@ -225,6 +225,120 @@
   </si>
   <si>
     <t>Leader</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Sidra</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Draper</t>
+  </si>
+  <si>
+    <t>Still</t>
+  </si>
+  <si>
+    <t>Dada</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Uland</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Mann</t>
+  </si>
+  <si>
+    <t>Saburo</t>
+  </si>
+  <si>
+    <t>Saito</t>
+  </si>
+  <si>
+    <t>Arnie</t>
+  </si>
+  <si>
+    <t>Saka</t>
+  </si>
+  <si>
+    <t>Tandon</t>
+  </si>
+  <si>
+    <t>Pam</t>
+  </si>
+  <si>
+    <t>Morton</t>
+  </si>
+  <si>
+    <t>Da-Xai</t>
+  </si>
+  <si>
+    <t>Dong</t>
+  </si>
+  <si>
+    <t>Penny</t>
+  </si>
+  <si>
+    <t>Daphne</t>
+  </si>
+  <si>
+    <t>Donegal</t>
+  </si>
+  <si>
+    <t>Dustan</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Thrifty Travel</t>
+  </si>
+  <si>
+    <t>Buckster</t>
+  </si>
+  <si>
+    <t>Molly Morph</t>
+  </si>
+  <si>
+    <t>Wonder Bread</t>
+  </si>
+  <si>
+    <t>np</t>
+  </si>
+  <si>
+    <t>Greeeting</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>go</t>
   </si>
 </sst>
 </file>
@@ -256,15 +370,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -281,11 +425,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -293,6 +446,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,31 +765,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
     <col min="7" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
     <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -618,8 +820,12 @@
       <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="29"/>
+      <c r="R1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -650,8 +856,27 @@
       <c r="N2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="29"/>
+      <c r="P2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -674,8 +899,15 @@
       <c r="N3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="29"/>
+      <c r="P3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -700,8 +932,19 @@
       <c r="N4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="29"/>
+      <c r="P4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="14"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -722,8 +965,19 @@
       <c r="N5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="29"/>
+      <c r="P5" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="28"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -747,8 +1001,19 @@
       <c r="N6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="29"/>
+      <c r="P6" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="18"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="27"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -771,75 +1036,129 @@
       <c r="N7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="29"/>
+      <c r="P7" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="N8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="29"/>
+      <c r="P8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="6"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>4</v>
+      <c r="G9" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>4</v>
+      <c r="J9" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>4</v>
+      <c r="M9" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="N9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="T9" s="8"/>
+      <c r="U9" s="9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="4"/>
       <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="29"/>
+      <c r="P10" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" s="23"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
@@ -855,15 +1174,28 @@
       <c r="N11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="29"/>
+      <c r="P11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11" s="16"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="27"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" t="s">
         <v>41</v>
       </c>
@@ -885,13 +1217,26 @@
       <c r="N12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="29"/>
+      <c r="P12" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="R12" s="16"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E13" t="s">
         <v>56</v>
       </c>
@@ -907,14 +1252,25 @@
       <c r="N13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="29"/>
+      <c r="P13" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" s="28"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="22"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
         <v>65</v>
@@ -931,14 +1287,21 @@
       <c r="N14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="29"/>
+      <c r="P14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
@@ -955,14 +1318,21 @@
       <c r="N15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="29"/>
+      <c r="P15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
         <v>66</v>
@@ -979,16 +1349,23 @@
       <c r="N16" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="29"/>
+      <c r="P16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1005,14 +1382,23 @@
       <c r="N17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1029,14 +1415,23 @@
       <c r="N18" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
         <v>55</v>
@@ -1050,8 +1445,13 @@
         <v>60</v>
       </c>
       <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="29"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
@@ -1064,34 +1464,41 @@
       </c>
       <c r="J20" s="4"/>
       <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="29"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="29"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="29"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="N13:N16">
-    <sortCondition ref="N13"/>
+  <sortState ref="P3:Q18">
+    <sortCondition ref="P3:P18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="83" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
14th - Comments finished, start on file upload
Bit more work on exceptional cases, e.g., for a new user who has no
Projects, Tickets or Comments
</commit_message>
<xml_diff>
--- a/BugTracker-classes.xlsx
+++ b/BugTracker-classes.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="22290" windowHeight="7710"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="22290" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Classes!$A$1:$V$23</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
   <si>
     <t>Ticket</t>
   </si>
@@ -339,13 +342,43 @@
   </si>
   <si>
     <t>go</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tpeara@gmail</t>
+  </si>
+  <si>
+    <t>tim@peara</t>
+  </si>
+  <si>
+    <t>Dorothy</t>
+  </si>
+  <si>
+    <t>Drucker</t>
+  </si>
+  <si>
+    <t>tim@theIonizer</t>
+  </si>
+  <si>
+    <t>Soloviev</t>
+  </si>
+  <si>
+    <t>Sasha</t>
+  </si>
+  <si>
+    <t>tp@face</t>
+  </si>
+  <si>
+    <t>IsArchived</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +398,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -435,10 +476,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,7 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -477,7 +518,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -485,8 +525,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -768,38 +816,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection sqref="A1:V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="1.42578125" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" customWidth="1"/>
     <col min="7" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="9" max="9" width="1.42578125" customWidth="1"/>
     <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="15" max="15" width="1.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.85546875" customWidth="1"/>
     <col min="21" max="21" width="8.5703125" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -820,12 +869,12 @@
       <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="29"/>
+      <c r="O1" s="27"/>
       <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -856,7 +905,7 @@
       <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="29"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="1" t="s">
         <v>95</v>
       </c>
@@ -875,8 +924,11 @@
       <c r="U2" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -899,15 +951,18 @@
       <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="29"/>
+      <c r="O3" s="27"/>
       <c r="P3" s="5" t="s">
         <v>79</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -932,19 +987,22 @@
       <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="29"/>
-      <c r="P4" s="10" t="s">
+      <c r="O4" s="27"/>
+      <c r="P4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="11"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="14"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R4" s="10"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -965,27 +1023,25 @@
       <c r="N5" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="19" t="s">
+      <c r="O5" s="27"/>
+      <c r="P5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="R5" s="28"/>
-      <c r="S5" s="20"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="19"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" t="s">
@@ -1001,28 +1057,30 @@
       <c r="N6" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="29"/>
-      <c r="P6" s="15" t="s">
+      <c r="O6" s="27"/>
+      <c r="P6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="18"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="27"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R6" s="17"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="25"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" t="s">
@@ -1036,30 +1094,28 @@
       <c r="N7" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="15" t="s">
+      <c r="O7" s="27"/>
+      <c r="P7" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R7" s="15"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>4</v>
@@ -1079,7 +1135,7 @@
       <c r="N8" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="29"/>
+      <c r="O8" s="27"/>
       <c r="P8" s="5" t="s">
         <v>90</v>
       </c>
@@ -1088,8 +1144,11 @@
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="7"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>101</v>
@@ -1120,7 +1179,7 @@
       <c r="N9" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="29"/>
+      <c r="O9" s="27"/>
       <c r="P9" s="5" t="s">
         <v>72</v>
       </c>
@@ -1128,30 +1187,28 @@
         <v>71</v>
       </c>
       <c r="T9" s="8"/>
-      <c r="U9" s="9"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U9" s="25"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="R10" s="23"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O10" s="27"/>
+      <c r="P10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="S10" s="7"/>
+      <c r="T10" s="24"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -1160,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="1" t="s">
@@ -1174,19 +1231,19 @@
       <c r="N11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q11" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="R11" s="16"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="27"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O11" s="27"/>
+      <c r="P11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -1197,7 +1254,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>3</v>
@@ -1217,19 +1274,19 @@
       <c r="N12" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q12" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="R12" s="16"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O12" s="27"/>
+      <c r="P12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="R12" s="15"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="25"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>25</v>
@@ -1238,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
@@ -1252,28 +1309,31 @@
       <c r="N13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="29"/>
-      <c r="P13" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="R13" s="28"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="22"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O13" s="27"/>
+      <c r="P13" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
@@ -1287,15 +1347,19 @@
       <c r="N14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O14" s="27"/>
+      <c r="P14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="R14" s="15"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="25"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>63</v>
@@ -1304,7 +1368,7 @@
         <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="2" t="s">
@@ -1318,15 +1382,18 @@
       <c r="N15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O15" s="27"/>
+      <c r="P15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q15" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="R15" s="26"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="20"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>103</v>
@@ -1335,7 +1402,7 @@
         <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="2" t="s">
@@ -1349,12 +1416,12 @@
       <c r="N16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O16" s="29"/>
+      <c r="O16" s="27"/>
       <c r="P16" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1368,7 +1435,7 @@
         <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="2" t="s">
@@ -1382,12 +1449,12 @@
       <c r="N17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O17" s="29"/>
+      <c r="O17" s="27"/>
       <c r="P17" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1401,7 +1468,7 @@
         <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="2" t="s">
@@ -1415,12 +1482,12 @@
       <c r="N18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O18" s="29"/>
+      <c r="O18" s="27"/>
       <c r="P18" s="5" t="s">
         <v>68</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1434,7 +1501,7 @@
         <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="2" t="s">
@@ -1445,7 +1512,13 @@
         <v>60</v>
       </c>
       <c r="M19" s="4"/>
-      <c r="O19" s="29"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -1453,10 +1526,10 @@
         <v>58</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="2" t="s">
@@ -1464,7 +1537,13 @@
       </c>
       <c r="J20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="O20" s="29"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -1475,30 +1554,45 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="O21" s="29"/>
+        <v>9</v>
+      </c>
+      <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="27"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
         <v>46</v>
       </c>
-      <c r="O22" s="29"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="4"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="P3:Q18">
-    <sortCondition ref="P3:P18"/>
+  <sortState ref="P16:V20">
+    <sortCondition ref="P16"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="V3" r:id="rId1"/>
+    <hyperlink ref="V4" r:id="rId2"/>
+    <hyperlink ref="V8" r:id="rId3"/>
+    <hyperlink ref="V13" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="83" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="79" orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>